<commit_message>
added new code and text
</commit_message>
<xml_diff>
--- a/PS-250/Lab4/Lab4_Work.xlsx
+++ b/PS-250/Lab4/Lab4_Work.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DevStark\Github\Fall_2018_Homework\PS-250\Lab4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84FF5AF9-F339-4575-A59C-333845D3E93D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FA25ADD-AD5C-44FF-97BE-4FB1D9ACFB38}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="900" windowWidth="25770" windowHeight="13560" activeTab="1" xr2:uid="{8FADD37C-FCA6-8C41-8761-D81F0C976274}"/>
+    <workbookView xWindow="0" yWindow="1350" windowWidth="25770" windowHeight="13560" xr2:uid="{8FADD37C-FCA6-8C41-8761-D81F0C976274}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3797,13 +3797,13 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>1328737</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>452437</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4202,8 +4202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E63EE814-A031-5F41-8CB1-158CBFFBE6E3}">
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -4795,6 +4795,10 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
+      <c r="H27" s="1">
+        <f>I2 / ((G21 / (2 * 3.14))^2) / 100</f>
+        <v>9.8350723731148815</v>
+      </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
@@ -5047,8 +5051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{428042F5-4FF8-407B-862A-BD5EBB764185}">
   <dimension ref="A1:K74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="E77" sqref="E77"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -5175,7 +5179,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
-        <f t="shared" ref="A31:B35" si="0">LN(A17)</f>
+        <f t="shared" ref="A31:B34" si="0">LN(A17)</f>
         <v>0.67294447324242579</v>
       </c>
       <c r="B31" s="1">

</xml_diff>